<commit_message>
scritti i nomi della colonna
</commit_message>
<xml_diff>
--- a/Database First.xlsx
+++ b/Database First.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\generation\Eserzcizi\SQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1BD198D8-C47A-42C4-89E0-8495D9484865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92F91EE-50A6-4EC6-B8B8-55962E02EA39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C5FA906F-871E-4E3E-A204-9B3F5AAE5935}"/>
   </bookViews>
@@ -33,10 +33,59 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>auto usate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nome Colonna : </t>
+  </si>
+  <si>
+    <t>Tipo di Dato :</t>
+  </si>
+  <si>
+    <t>Chiave Primaria :</t>
+  </si>
+  <si>
+    <t>modello</t>
+  </si>
+  <si>
+    <t>porte</t>
+  </si>
+  <si>
+    <t>numero_Sedie</t>
+  </si>
+  <si>
+    <t>targa</t>
+  </si>
+  <si>
+    <t>numero_proprietari_precendti</t>
+  </si>
+  <si>
+    <t>cilindrata</t>
+  </si>
+  <si>
+    <t>uso_commerciale</t>
+  </si>
+  <si>
+    <t>motore_originale</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -64,8 +113,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -380,12 +430,75 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11C2B162-FABE-490F-9109-34120CD40DC2}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="28.140625" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
DICHIARATI I TIPI DI DATI
</commit_message>
<xml_diff>
--- a/Database First.xlsx
+++ b/Database First.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\generation\Eserzcizi\SQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92F91EE-50A6-4EC6-B8B8-55962E02EA39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CEAC560-7AFF-4CCF-8595-1F4F188178E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C5FA906F-871E-4E3E-A204-9B3F5AAE5935}"/>
+    <workbookView xWindow="7275" yWindow="6330" windowWidth="21600" windowHeight="11505" xr2:uid="{C5FA906F-871E-4E3E-A204-9B3F5AAE5935}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>auto usate</t>
   </si>
@@ -70,6 +70,21 @@
   </si>
   <si>
     <t>motore_originale</t>
+  </si>
+  <si>
+    <t>VARCHAR(100)</t>
+  </si>
+  <si>
+    <t>TINYINT</t>
+  </si>
+  <si>
+    <t>CHAR(7)</t>
+  </si>
+  <si>
+    <t>SMALLINT</t>
+  </si>
+  <si>
+    <t>BOOL</t>
   </si>
 </sst>
 </file>
@@ -433,12 +448,13 @@
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" customWidth="1"/>
     <col min="6" max="6" width="28.140625" customWidth="1"/>
     <col min="8" max="8" width="16.140625" customWidth="1"/>
@@ -491,6 +507,30 @@
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">

</xml_diff>

<commit_message>
DICHIARATA TARGA COME CHIAVE PRIMARIA
</commit_message>
<xml_diff>
--- a/Database First.xlsx
+++ b/Database First.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\generation\Eserzcizi\SQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CEAC560-7AFF-4CCF-8595-1F4F188178E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2940CDC6-B123-416B-B6B9-F8FF0E3F7BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7275" yWindow="6330" windowWidth="21600" windowHeight="11505" xr2:uid="{C5FA906F-871E-4E3E-A204-9B3F5AAE5935}"/>
+    <workbookView xWindow="12960" yWindow="2985" windowWidth="21600" windowHeight="11505" xr2:uid="{C5FA906F-871E-4E3E-A204-9B3F5AAE5935}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>auto usate</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>BOOL</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -448,7 +451,7 @@
   <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,6 +539,9 @@
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>